<commit_message>
06/28 test result README update
</commit_message>
<xml_diff>
--- a/test_result.xlsx
+++ b/test_result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김수환\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김수환\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu20.04onWindows_79rhkp1fndgsc\LocalState\rootfs\home\susoon\work\Research_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A037CA89-EF5C-4929-B79F-81B25DDF391F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AE51C1-1BD5-4BED-B257-6A2BDCEF1120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB014DAC-0EAB-4ABD-951C-D114096D7E56}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>access</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,6 +102,15 @@
     <t>percentage-max</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>percentage-avg</t>
+  </si>
+  <si>
+    <t>percentage-min</t>
+  </si>
+  <si>
+    <t>percentage-max</t>
+  </si>
 </sst>
 </file>
 
@@ -168,6 +177,927 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>percentage-avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$I$17:$J$25</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>access</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>memcpy</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>add</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>access</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>memcpy</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>add</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>access</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>memcpy</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>add</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>OFF</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>DPDK</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>GPU-Ether</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$17:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0821237549211746</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1770639417698243</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0851152675795461</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0056371130134418</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.02493141708828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0046966990805053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-152C-4D9A-B14E-12E55B93A1F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2093507535"/>
+        <c:axId val="2093751167"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2093507535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2093751167"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2093751167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2093507535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>194310</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="차트 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5216D135-3ABE-4106-835B-5C76B9AFE3C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B7BC6B-844A-44C8-AF2B-4F92E3590E11}">
-  <dimension ref="A4:M13"/>
+  <dimension ref="A4:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -551,15 +1481,15 @@
         <v>208034</v>
       </c>
       <c r="K5">
-        <f>H$5/H5</f>
+        <f>H5/H$5</f>
         <v>1</v>
       </c>
       <c r="L5">
-        <f>I$5/I5</f>
+        <f t="shared" ref="L5:M5" si="0">I5/I$5</f>
         <v>1</v>
       </c>
       <c r="M5">
-        <f>J$5/J5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -584,27 +1514,27 @@
         <v>133765</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H7" si="0">AVERAGE(C6:G6)</f>
+        <f t="shared" ref="H6:H7" si="1">AVERAGE(C6:G6)</f>
         <v>132467.4</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I7" si="1">MIN(C6:G6)</f>
+        <f t="shared" ref="I6:I7" si="2">MIN(C6:G6)</f>
         <v>131471</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J7" si="2">MAX(C6:G6)</f>
+        <f t="shared" ref="J6:J7" si="3">MAX(C6:G6)</f>
         <v>133765</v>
       </c>
       <c r="K6">
-        <f>H$6/H6</f>
+        <f>H6/H$6</f>
         <v>1</v>
       </c>
       <c r="L6">
-        <f>I$6/I6</f>
+        <f t="shared" ref="L6:M6" si="4">I6/I$6</f>
         <v>1</v>
       </c>
       <c r="M6">
-        <f>J$6/J6</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -629,27 +1559,27 @@
         <v>96789</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>96748.800000000003</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96642</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96847</v>
       </c>
       <c r="K7">
-        <f>H$7/H7</f>
+        <f>H7/H$7</f>
         <v>1</v>
       </c>
       <c r="L7">
-        <f>I$7/I7</f>
+        <f t="shared" ref="L7:M7" si="5">I7/I$7</f>
         <v>1</v>
       </c>
       <c r="M7">
-        <f>J$7/J7</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -688,16 +1618,16 @@
         <v>225082</v>
       </c>
       <c r="K8">
-        <f>H$5/H8</f>
-        <v>0.92410872180958936</v>
+        <f>H8/H$5</f>
+        <v>1.0821237549211746</v>
       </c>
       <c r="L8">
-        <f>I$5/I8</f>
-        <v>0.92393424847464101</v>
+        <f t="shared" ref="L8:M8" si="6">I8/I$5</f>
+        <v>1.0823281003501481</v>
       </c>
       <c r="M8">
-        <f>J$5/J8</f>
-        <v>0.92425871460178954</v>
+        <f t="shared" si="6"/>
+        <v>1.0819481430919946</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
@@ -721,28 +1651,28 @@
         <v>158272</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H10" si="3">AVERAGE(C9:G9)</f>
+        <f t="shared" ref="H9:H10" si="7">AVERAGE(C9:G9)</f>
         <v>155922.6</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I10" si="4">MIN(C9:G9)</f>
+        <f t="shared" ref="I9:I10" si="8">MIN(C9:G9)</f>
         <v>153939</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9:J10" si="5">MAX(C9:G9)</f>
+        <f t="shared" ref="J9:J10" si="9">MAX(C9:G9)</f>
         <v>158272</v>
       </c>
       <c r="K9">
-        <f>H$6/H9</f>
-        <v>0.84957151817632592</v>
+        <f>H9/H$6</f>
+        <v>1.1770639417698243</v>
       </c>
       <c r="L9">
-        <f>I$6/I9</f>
-        <v>0.8540460831887956</v>
+        <f t="shared" ref="L9:M9" si="10">I9/I$6</f>
+        <v>1.1708970039020012</v>
       </c>
       <c r="M9">
-        <f>J$6/J9</f>
-        <v>0.8451589668418924</v>
+        <f t="shared" si="10"/>
+        <v>1.1832093596979778</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
@@ -766,28 +1696,28 @@
         <v>105023</v>
       </c>
       <c r="H10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>104983.6</v>
       </c>
       <c r="I10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>104779</v>
       </c>
       <c r="J10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>105332</v>
       </c>
       <c r="K10">
-        <f>H$7/H10</f>
-        <v>0.92156108192136676</v>
+        <f>H10/H$7</f>
+        <v>1.0851152675795461</v>
       </c>
       <c r="L10">
-        <f>I$7/I10</f>
-        <v>0.92234130885005583</v>
+        <f t="shared" ref="L10:M10" si="11">I10/I$7</f>
+        <v>1.0841973469092112</v>
       </c>
       <c r="M10">
-        <f>J$7/J10</f>
-        <v>0.91944518285041588</v>
+        <f t="shared" si="11"/>
+        <v>1.0876124195896621</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
@@ -825,16 +1755,16 @@
         <v>209243</v>
       </c>
       <c r="K11">
-        <f>H$5/H11</f>
-        <v>0.99439448590302126</v>
+        <f>H11/H$5</f>
+        <v>1.0056371130134418</v>
       </c>
       <c r="L11">
-        <f>I$5/I11</f>
-        <v>0.99450875346790391</v>
+        <f t="shared" ref="L11:M11" si="12">I11/I$5</f>
+        <v>1.0055215668167301</v>
       </c>
       <c r="M11">
-        <f>J$5/J11</f>
-        <v>0.99422202893286749</v>
+        <f t="shared" si="12"/>
+        <v>1.0058115500350904</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
@@ -858,28 +1788,28 @@
         <v>134589</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:H13" si="6">AVERAGE(C12:G12)</f>
+        <f t="shared" ref="H12:H13" si="13">AVERAGE(C12:G12)</f>
         <v>135770</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I13" si="7">MIN(C12:G12)</f>
+        <f t="shared" ref="I12:I13" si="14">MIN(C12:G12)</f>
         <v>133920</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J13" si="8">MAX(C12:G12)</f>
+        <f t="shared" ref="J12:J13" si="15">MAX(C12:G12)</f>
         <v>138958</v>
       </c>
       <c r="K12">
-        <f>H$6/H12</f>
-        <v>0.97567503866833616</v>
+        <f>H12/H$6</f>
+        <v>1.02493141708828</v>
       </c>
       <c r="L12">
-        <f>I$6/I12</f>
-        <v>0.98171296296296295</v>
+        <f t="shared" ref="L12:M12" si="16">I12/I$6</f>
+        <v>1.0186276821504363</v>
       </c>
       <c r="M12">
-        <f>J$6/J12</f>
-        <v>0.96262899581168415</v>
+        <f t="shared" si="16"/>
+        <v>1.0388218143759578</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -903,38 +1833,194 @@
         <v>97070</v>
       </c>
       <c r="H13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>97203.199999999997</v>
       </c>
       <c r="I13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>97070</v>
       </c>
       <c r="J13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="15"/>
         <v>97321</v>
       </c>
       <c r="K13">
-        <f>H$7/H13</f>
-        <v>0.99532525678166983</v>
+        <f>H13/H$7</f>
+        <v>1.0046966990805053</v>
       </c>
       <c r="L13">
-        <f>I$7/I13</f>
-        <v>0.99559081075512512</v>
+        <f t="shared" ref="L13:M13" si="17">I13/I$7</f>
+        <v>1.0044287162931231</v>
       </c>
       <c r="M13">
-        <f>J$7/J13</f>
-        <v>0.99512951983641762</v>
+        <f t="shared" si="17"/>
+        <v>1.0048943178415439</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="K16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I18" s="1"/>
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I19" s="1"/>
+      <c r="J19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1.0821237549211746</v>
+      </c>
+      <c r="L20">
+        <v>1.0823281003501481</v>
+      </c>
+      <c r="M20">
+        <v>1.0819481430919946</v>
+      </c>
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I21" s="1"/>
+      <c r="J21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1.1770639417698243</v>
+      </c>
+      <c r="L21">
+        <v>1.1708970039020012</v>
+      </c>
+      <c r="M21">
+        <v>1.1832093596979778</v>
+      </c>
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I22" s="1"/>
+      <c r="J22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>1.0851152675795461</v>
+      </c>
+      <c r="L22">
+        <v>1.0841973469092112</v>
+      </c>
+      <c r="M22">
+        <v>1.0876124195896621</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1.0056371130134418</v>
+      </c>
+      <c r="L23">
+        <v>1.0055215668167301</v>
+      </c>
+      <c r="M23">
+        <v>1.0058115500350904</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I24" s="1"/>
+      <c r="J24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1.02493141708828</v>
+      </c>
+      <c r="L24">
+        <v>1.0186276821504363</v>
+      </c>
+      <c r="M24">
+        <v>1.0388218143759578</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.4">
+      <c r="I25" s="1"/>
+      <c r="J25" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>1.0046966990805053</v>
+      </c>
+      <c r="L25">
+        <v>1.0044287162931231</v>
+      </c>
+      <c r="M25">
+        <v>1.0048943178415439</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="I23:I25"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="I20:I22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
07/08 dpdk design update
</commit_message>
<xml_diff>
--- a/test_result.xlsx
+++ b/test_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김수환\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu20.04onWindows_79rhkp1fndgsc\LocalState\rootfs\home\susoon\work\Research_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F2AF79-CBA5-4A80-ACDE-EEB3DE448F70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93522EC-BA57-47B9-B773-33F385D8B002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FB014DAC-0EAB-4ABD-951C-D114096D7E56}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>access</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,6 +148,34 @@
     <t>router</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>IPSec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NIDS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPv4 Forwarding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add 2 arrays</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access 1 array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memcpy array to another array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -192,15 +220,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -233,37 +267,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ko-KR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -275,11 +279,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$16</c:f>
+              <c:f>Sheet1!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>percentage-avg</c:v>
+                  <c:v>Idle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -289,65 +293,94 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Sheet1!$I$17:$J$25</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="9"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>access</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>memcpy</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>add</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>access</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>memcpy</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>add</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>access</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>memcpy</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>add</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>OFF</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>DPDK</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>GPU-Ether</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Access 1 array</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add 2 arrays</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Memcpy array to another array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$17:$K$25</c:f>
+              <c:f>Sheet1!$C$18:$E$18</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -356,37 +389,270 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0821237549211746</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1770639417698243</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0851152675795461</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0056371130134418</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.02493141708828</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0046966990805053</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-152C-4D9A-B14E-12E55B93A1F7}"/>
+              <c16:uniqueId val="{00000000-F72D-4971-A55B-740A4459C36D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DPDK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Access 1 array</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add 2 arrays</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Memcpy array to another array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$20:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0823281003501481</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0841973469092112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1708970039020012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F72D-4971-A55B-740A4459C36D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GPU-Ether</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Access 1 array</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add 2 arrays</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Memcpy array to another array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0055215668167301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0044287162931231</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0186276821504363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F72D-4971-A55B-740A4459C36D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -394,16 +660,76 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2093507535"/>
-        <c:axId val="2093751167"/>
+        <c:axId val="2090120336"/>
+        <c:axId val="71850848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2093507535"/>
+        <c:axId val="2090120336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1"/>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0"/>
+                  <a:t> Case</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR" altLang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -441,7 +767,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093751167"/>
+        <c:crossAx val="71850848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -449,7 +775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093751167"/>
+        <c:axId val="71850848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,7 +795,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0"/>
+                  <a:t>Latency Increment ( Idle / app )</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR" altLang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -500,7 +882,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2093507535"/>
+        <c:crossAx val="2090120336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -512,6 +894,1416 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Idle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Access 1 array</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add 2 arrays</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Memcpy array to another array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$18:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E7C-4BE8-AB6B-90104AED3621}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GPU-Ether</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Access 1 array</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add 2 arrays</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Memcpy array to another array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0055215668167301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0044287162931231</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0186276821504363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8E7C-4BE8-AB6B-90104AED3621}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DPDK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Access 1 array</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add 2 arrays</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Memcpy array to another array</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$20:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0823281003501481</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0841973469092112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1708970039020012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8E7C-4BE8-AB6B-90104AED3621}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="1160280272"/>
+        <c:axId val="1361479632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1160280272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" sz="1000" b="1" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Test Case</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR" altLang="ko-KR">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1361479632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1361479632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" sz="1000" b="1" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Latency Increment ( Idle / app )</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR" altLang="ko-KR">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1160280272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IPSec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ko-KR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$H$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.3860000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9729999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1309999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2549999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-92F1-405E-A60F-864E77862AB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NIDS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$H$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$4:$M$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-92F1-405E-A60F-864E77862AB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IPv4 Forwarding</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$H$2:$M$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$H$5:$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-92F1-405E-A60F-864E77862AB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="2079995440"/>
+        <c:axId val="71857088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2079995440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1"/>
+                  <a:t>Packet</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0"/>
+                  <a:t> Size ( bytes )</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR" altLang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71857088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71857088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1"/>
+                  <a:t>Throughput</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" b="1" baseline="0"/>
+                  <a:t> ( Gbps )</a:t>
+                </a:r>
+                <a:endParaRPr lang="ko-KR" altLang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ko-KR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2079995440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -596,6 +2388,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1099,27 +2971,1110 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>422910</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B96EA2B5-BCE1-4235-87C3-666C4B2F8C55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>346710</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>201930</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>110490</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="차트 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{879CDF2F-FE2F-4880-9956-A0A864E8681B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>758190</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="차트 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5216D135-3ABE-4106-835B-5C76B9AFE3C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32F67272-266B-405E-A074-7243A7A76970}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,10 +4392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B7BC6B-844A-44C8-AF2B-4F92E3590E11}">
-  <dimension ref="A4:M25"/>
+  <dimension ref="A4:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1487,7 +4442,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
@@ -1534,7 +4489,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="1"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1579,7 +4534,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="1"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1624,7 +4579,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
@@ -1671,7 +4626,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="1"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1716,7 +4671,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A10" s="1"/>
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -1761,7 +4716,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
@@ -1808,7 +4763,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="1"/>
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -1853,7 +4808,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="1"/>
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1908,146 +4863,207 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I17" s="1" t="s">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J17" t="s">
         <v>0</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>1</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <v>1</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I18" s="1"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3">
+        <f>L5</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <f>L7</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <f>L6</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <v>1</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <v>1</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I19" s="1"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3">
+        <f>L11</f>
+        <v>1.0055215668167301</v>
+      </c>
+      <c r="D19" s="3">
+        <f>L13</f>
+        <v>1.0044287162931231</v>
+      </c>
+      <c r="E19" s="3">
+        <f>L12</f>
+        <v>1.0186276821504363</v>
+      </c>
+      <c r="I19" s="4"/>
       <c r="J19" t="s">
         <v>2</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K19" s="1">
         <v>1</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="1">
         <v>1</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I20" s="1" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3">
+        <f>L8</f>
+        <v>1.0823281003501481</v>
+      </c>
+      <c r="D20" s="3">
+        <f>L10</f>
+        <v>1.0841973469092112</v>
+      </c>
+      <c r="E20" s="3">
+        <f>L9</f>
+        <v>1.1708970039020012</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J20" t="s">
         <v>0</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="1">
         <v>1.0821237549211746</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="1">
         <v>1.0823281003501481</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="1">
         <v>1.0819481430919946</v>
       </c>
     </row>
-    <row r="21" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I21" s="1"/>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="I21" s="4"/>
       <c r="J21" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>1.1770639417698243</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="1">
         <v>1.1708970039020012</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="1">
         <v>1.1832093596979778</v>
       </c>
     </row>
-    <row r="22" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I22" s="1"/>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C22" s="1"/>
+      <c r="I22" s="4"/>
       <c r="J22" t="s">
         <v>2</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>1.0851152675795461</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="1">
         <v>1.0841973469092112</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="1">
         <v>1.0876124195896621</v>
       </c>
     </row>
-    <row r="23" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I23" s="1" t="s">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C23" s="1"/>
+      <c r="I23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J23" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>1.0056371130134418</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="1">
         <v>1.0055215668167301</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="1">
         <v>1.0058115500350904</v>
       </c>
     </row>
-    <row r="24" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I24" s="1"/>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C24" s="1"/>
+      <c r="I24" s="4"/>
       <c r="J24" t="s">
         <v>1</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>1.02493141708828</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="1">
         <v>1.0186276821504363</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="1">
         <v>1.0388218143759578</v>
       </c>
     </row>
-    <row r="25" spans="9:13" x14ac:dyDescent="0.4">
-      <c r="I25" s="1"/>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C25" s="1"/>
+      <c r="I25" s="4"/>
       <c r="J25" t="s">
         <v>2</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>1.0046966990805053</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="1">
         <v>1.0044287162931231</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <v>1.0048943178415439</v>
       </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="C26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2067,20 +5083,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFCDDB8-F918-42FA-B80B-15D297F84878}">
-  <dimension ref="B2:D26"/>
+  <dimension ref="B2:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="7" width="16.796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C2" t="s">
         <v>26</v>
       </c>
+      <c r="H2">
+        <v>64</v>
+      </c>
+      <c r="I2">
+        <v>128</v>
+      </c>
+      <c r="J2">
+        <v>256</v>
+      </c>
+      <c r="K2">
+        <v>512</v>
+      </c>
+      <c r="L2">
+        <v>1024</v>
+      </c>
+      <c r="M2">
+        <v>1514</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -2090,8 +5127,29 @@
       <c r="D3">
         <v>2.3860000000000001</v>
       </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2.3860000000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2.9729999999999999</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3.1309999999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3.2549999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -2101,8 +5159,29 @@
       <c r="D4">
         <v>2.7309999999999999</v>
       </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2">
+        <v>10</v>
+      </c>
+      <c r="L4" s="2">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -2112,8 +5191,29 @@
       <c r="D5">
         <v>2.9729999999999999</v>
       </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2">
+        <v>10</v>
+      </c>
+      <c r="L5" s="2">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>23</v>
       </c>
@@ -2124,7 +5224,7 @@
         <v>3.1309999999999998</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -2135,7 +5235,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -2146,12 +5246,12 @@
         <v>3.2549999999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -2162,24 +5262,48 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>21</v>
       </c>
+      <c r="C13">
+        <v>8446</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>22</v>
       </c>
+      <c r="C14">
+        <v>4529</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>23</v>
       </c>
+      <c r="C15">
+        <v>2345</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>24</v>
+      </c>
+      <c r="C16">
+        <v>1195</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.4">
@@ -2267,5 +5391,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
07/14 DPDK I/O and GPU-Ether NF test result
</commit_message>
<xml_diff>
--- a/test_result.xlsx
+++ b/test_result.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김수환\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu20.04onWindows_79rhkp1fndgsc\LocalState\rootfs\home\susoon\work\Research_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93522EC-BA57-47B9-B773-33F385D8B002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CA79E5-8AC9-443B-BBB3-4C3F636AE8B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{FB014DAC-0EAB-4ABD-951C-D114096D7E56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{FB014DAC-0EAB-4ABD-951C-D114096D7E56}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="cache pollution" sheetId="1" r:id="rId1"/>
+    <sheet name="07.04 nf-GPU-ETHER" sheetId="2" r:id="rId2"/>
+    <sheet name="DPDK without GPU" sheetId="3" r:id="rId3"/>
+    <sheet name="07.14 GPU-Ether nf" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="38">
   <si>
     <t>access</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,6 +178,14 @@
     <t>Memcpy array to another array</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>No Opt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">O3 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +289,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>'cache pollution'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -360,7 +370,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:f>'cache pollution'!$C$17:$E$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -377,7 +387,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$E$18</c:f>
+              <c:f>'cache pollution'!$C$18:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -404,7 +414,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
+              <c:f>'cache pollution'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -485,7 +495,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:f>'cache pollution'!$C$17:$E$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -502,7 +512,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$E$20</c:f>
+              <c:f>'cache pollution'!$C$20:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -529,7 +539,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$19</c:f>
+              <c:f>'cache pollution'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -610,7 +620,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:f>'cache pollution'!$C$17:$E$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -627,7 +637,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$E$19</c:f>
+              <c:f>'cache pollution'!$C$19:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -990,7 +1000,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>'cache pollution'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1071,7 +1081,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:f>'cache pollution'!$C$17:$E$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1088,7 +1098,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$E$18</c:f>
+              <c:f>'cache pollution'!$C$18:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1115,7 +1125,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$19</c:f>
+              <c:f>'cache pollution'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1196,7 +1206,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:f>'cache pollution'!$C$17:$E$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1213,7 +1223,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$E$19</c:f>
+              <c:f>'cache pollution'!$C$19:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1240,7 +1250,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$20</c:f>
+              <c:f>'cache pollution'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1321,7 +1331,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$17:$E$17</c:f>
+              <c:f>'cache pollution'!$C$17:$E$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1338,7 +1348,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$E$20</c:f>
+              <c:f>'cache pollution'!$C$20:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1715,7 +1725,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$3</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1795,7 +1805,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$H$2:$M$2</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$H$2:$M$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1822,7 +1832,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$H$3:$M$3</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$H$3:$M$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1858,7 +1868,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$4</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1881,7 +1891,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$H$2:$M$2</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$H$2:$M$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1908,7 +1918,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$H$4:$M$4</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$H$4:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1944,7 +1954,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$G$5</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$G$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1967,7 +1977,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$H$2:$M$2</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$H$2:$M$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1994,7 +2004,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$H$5:$M$5</c:f>
+              <c:f>'07.04 nf-GPU-ETHER'!$H$5:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2348,6 +2358,397 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DPDK without GPU'!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Opt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'DPDK without GPU'!$F$4:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'DPDK without GPU'!$G$4:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.81097099101035219</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99999650896497794</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99999787193564049</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99999177920253335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0000012272378067</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-71A2-4455-8948-EB55E59629D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DPDK without GPU'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O3 </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'DPDK without GPU'!$F$4:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64B</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128B</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>256B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024B</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1514B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'DPDK without GPU'!$H$4:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0000015456489613</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99999602064116833</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99999293417454926</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000029792989795</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0000041104223869</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-71A2-4455-8948-EB55E59629D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="75147712"/>
+        <c:axId val="1897551536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75147712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1897551536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1897551536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="75147712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2468,6 +2869,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3475,6 +3916,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4075,6 +5019,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32F67272-266B-405E-A074-7243A7A76970}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>407670</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56CC40B-17C6-4885-BC8C-1EB22B33AC54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4394,7 +5379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B7BC6B-844A-44C8-AF2B-4F92E3590E11}">
   <dimension ref="A4:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
@@ -5085,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFCDDB8-F918-42FA-B80B-15D297F84878}">
   <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5393,4 +6378,701 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CB2661-8C9B-4E7C-AD51-D3899A48BE22}">
+  <dimension ref="B3:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>12256516</v>
+      </c>
+      <c r="D4">
+        <v>14880504</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1">
+        <f>C4/15113384</f>
+        <v>0.81097099101035219</v>
+      </c>
+      <c r="H4" s="1">
+        <f>D4/14880481</f>
+        <v>1.0000015456489613</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>8510000</v>
+      </c>
+      <c r="D5">
+        <v>8544056</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <f>C5/8510000</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <f>D5/8544090</f>
+        <v>0.99999602064116833</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>4583152</v>
+      </c>
+      <c r="D6">
+        <v>4528809</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="1">
+        <f>C6/4583168</f>
+        <v>0.99999650896497794</v>
+      </c>
+      <c r="H6" s="1">
+        <f>D6/4528841</f>
+        <v>0.99999293417454926</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>2349548</v>
+      </c>
+      <c r="D7">
+        <v>2349553</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1">
+        <f>C7/2349553</f>
+        <v>0.99999787193564049</v>
+      </c>
+      <c r="H7" s="1">
+        <f>D7/2349546</f>
+        <v>1.0000029792989795</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>1216417</v>
+      </c>
+      <c r="D8">
+        <v>1216425</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1">
+        <f>C8/1216427</f>
+        <v>0.99999177920253335</v>
+      </c>
+      <c r="H8" s="1">
+        <f>D8/1216420</f>
+        <v>1.0000041104223869</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>814839</v>
+      </c>
+      <c r="D9">
+        <v>818092</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1">
+        <f>C9/814838</f>
+        <v>1.0000012272378067</v>
+      </c>
+      <c r="H9" s="1">
+        <f>D9/818092</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8385EA-C2DC-4E14-97DF-A69252E9ABC7}">
+  <dimension ref="B4:O28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="8" width="9.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>8.7140000000000004</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>13028884</v>
+      </c>
+      <c r="H14">
+        <v>14936543</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1">
+        <f>C14/D14</f>
+        <v>0.87140000000000006</v>
+      </c>
+      <c r="N14" t="s">
+        <v>20</v>
+      </c>
+      <c r="O14" s="1">
+        <f>G14/H14</f>
+        <v>0.87228242840394865</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>9.9979999999999993</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15">
+        <v>8443822</v>
+      </c>
+      <c r="H15">
+        <v>8443774</v>
+      </c>
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" ref="K15:K19" si="0">C15/D15</f>
+        <v>0.99979999999999991</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" ref="O15:O19" si="1">G15/H15</f>
+        <v>1.0000056846618586</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16">
+        <v>4528849</v>
+      </c>
+      <c r="H16">
+        <v>4528846</v>
+      </c>
+      <c r="J16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0000006624204048</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17">
+        <v>2387106</v>
+      </c>
+      <c r="H17">
+        <v>2387104</v>
+      </c>
+      <c r="J17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0000008378353016</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18">
+        <v>1197277</v>
+      </c>
+      <c r="H18">
+        <v>1197279</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.99999832954557788</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19">
+        <v>818091</v>
+      </c>
+      <c r="H19">
+        <v>818091</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>8.7110000000000003</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <v>13392640</v>
+      </c>
+      <c r="H23">
+        <v>15116035</v>
+      </c>
+      <c r="J23" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="1">
+        <f>C23/D23</f>
+        <v>0.87109999999999999</v>
+      </c>
+      <c r="N23" t="s">
+        <v>20</v>
+      </c>
+      <c r="O23" s="1">
+        <f>G23/H23</f>
+        <v>0.88598895146776258</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>9.9979999999999993</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24">
+        <v>8443979</v>
+      </c>
+      <c r="H24">
+        <v>8443975</v>
+      </c>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" ref="K24:K28" si="2">C24/D24</f>
+        <v>0.99979999999999991</v>
+      </c>
+      <c r="N24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" ref="O24:O28" si="3">G24/H24</f>
+        <v>1.000000473710545</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25">
+        <v>4528853</v>
+      </c>
+      <c r="H25">
+        <v>4528839</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000030912999998</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26">
+        <v>2349549</v>
+      </c>
+      <c r="H26">
+        <v>2349538</v>
+      </c>
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000046817714803</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27">
+        <v>1197281</v>
+      </c>
+      <c r="H27">
+        <v>1197278</v>
+      </c>
+      <c r="J27" t="s">
+        <v>24</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>24</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000025056837258</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <v>814839</v>
+      </c>
+      <c r="H28">
+        <v>814837</v>
+      </c>
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>25</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0000024544786257</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
07/16 NIDS and Router Evaluation with Random Pkt
</commit_message>
<xml_diff>
--- a/test_result.xlsx
+++ b/test_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김수환\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu20.04onWindows_79rhkp1fndgsc\LocalState\rootfs\home\susoon\work\Research_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CA79E5-8AC9-443B-BBB3-4C3F636AE8B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725A21DB-1FAA-4B98-BD6F-112AB0000B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{FB014DAC-0EAB-4ABD-951C-D114096D7E56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{FB014DAC-0EAB-4ABD-951C-D114096D7E56}"/>
   </bookViews>
   <sheets>
     <sheet name="cache pollution" sheetId="1" r:id="rId1"/>
@@ -5379,8 +5379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B7BC6B-844A-44C8-AF2B-4F92E3590E11}">
   <dimension ref="A4:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6070,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFCDDB8-F918-42FA-B80B-15D297F84878}">
   <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6376,7 +6376,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6385,7 +6386,7 @@
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6543,7 +6544,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6551,8 +6553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D8385EA-C2DC-4E14-97DF-A69252E9ABC7}">
   <dimension ref="B4:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>